<commit_message>
att bd e cronograma
</commit_message>
<xml_diff>
--- a/.outros/Documentos/CRONOGRAMA - PROJETO ATHENA.xlsx
+++ b/.outros/Documentos/CRONOGRAMA - PROJETO ATHENA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php\projeto-athena\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php\projeto-athena\.outros\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95454AF-C390-4B3D-AA0D-043B77076E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A070A27A-166A-4A05-A9F1-3AED695E77DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9984709C-C237-45B3-B008-D2F69F35A1CE}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{9984709C-C237-45B3-B008-D2F69F35A1CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -118,7 +118,7 @@
     <t>APRESENTAÇÃO</t>
   </si>
   <si>
-    <t>EQUIPE: WARRIORS.NET</t>
+    <t>EQUIPE: WARRIORS NET</t>
   </si>
 </sst>
 </file>
@@ -783,7 +783,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1143,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
       <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="N17" s="25"/>
       <c r="O17" s="25"/>
     </row>
   </sheetData>

</xml_diff>